<commit_message>
change of Project Structure
</commit_message>
<xml_diff>
--- a/projects/DriveMaster/reports/permissions_editor.xlsx
+++ b/projects/DriveMaster/reports/permissions_editor.xlsx
@@ -64,6 +64,32 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8E9BB"/>
+          <bgColor rgb="FFD8E9BB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -425,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,34 +512,34 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Add_Principal_Type</t>
+          <t>Type (for ADD)</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Add_Principal_Address</t>
+          <t>Email/Domain (for ADD)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>/Python_Admin_Tool_TESTING/Test Doc 1</t>
+          <t>/Python_Admin_Tool_TESTING/Sub-Folder 1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Test Doc 1</t>
+          <t>Sub-Folder 1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1O90b5jSuK3lIz-RYZIEtAAlA3-IQ_vmxgulyB_6vY2U</t>
+          <t>1jPqgww8lNGleK7h15iHuNdyUbZDf0idz</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Viewer</t>
+          <t>Commenter</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -533,29 +559,29 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://docs.google.com/document/d/1O90b5jSuK3lIz-RYZIEtAAlA3-IQ_vmxgulyB_6vY2U/edit?usp=drivesdk</t>
+          <t>https://drive.google.com/drive/folders/1jPqgww8lNGleK7h15iHuNdyUbZDf0idz</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>/Python_Admin_Tool_TESTING/Test Doc 1</t>
+          <t>/Python_Admin_Tool_TESTING/Sub-Folder 1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Test Doc 1</t>
+          <t>Sub-Folder 1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1O90b5jSuK3lIz-RYZIEtAAlA3-IQ_vmxgulyB_6vY2U</t>
+          <t>1jPqgww8lNGleK7h15iHuNdyUbZDf0idz</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Editor</t>
+          <t>Viewer</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -575,24 +601,24 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://docs.google.com/document/d/1O90b5jSuK3lIz-RYZIEtAAlA3-IQ_vmxgulyB_6vY2U/edit?usp=drivesdk</t>
+          <t>https://drive.google.com/drive/folders/1jPqgww8lNGleK7h15iHuNdyUbZDf0idz</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>/Python_Admin_Tool_TESTING/Test Doc 1</t>
+          <t>/Python_Admin_Tool_TESTING/Sub-Folder 1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Test Doc 1</t>
+          <t>Sub-Folder 1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1O90b5jSuK3lIz-RYZIEtAAlA3-IQ_vmxgulyB_6vY2U</t>
+          <t>1jPqgww8lNGleK7h15iHuNdyUbZDf0idz</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -617,39 +643,39 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://docs.google.com/document/d/1O90b5jSuK3lIz-RYZIEtAAlA3-IQ_vmxgulyB_6vY2U/edit?usp=drivesdk</t>
+          <t>https://drive.google.com/drive/folders/1jPqgww8lNGleK7h15iHuNdyUbZDf0idz</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>/Python_Admin_Tool_TESTING/Sub-Folder 1</t>
+          <t>/Python_Admin_Tool_TESTING/Sub-Folder 1/Test Sheet 2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sub-Folder 1</t>
+          <t>Test Sheet 2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1jPqgww8lNGleK7h15iHuNdyUbZDf0idz</t>
+          <t>1Wan1C_Cxndc2M6yXKa8vxJLXCgYoBXFzDVwRYAfGbVY</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Viewer</t>
+          <t>Editor</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>domain</t>
+          <t>group</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>bioaccessla.com</t>
+          <t>jesus_test_group@bioaccessla.com</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -659,39 +685,39 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1jPqgww8lNGleK7h15iHuNdyUbZDf0idz</t>
+          <t>https://docs.google.com/spreadsheets/d/1Wan1C_Cxndc2M6yXKa8vxJLXCgYoBXFzDVwRYAfGbVY/edit?usp=drivesdk</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>/Python_Admin_Tool_TESTING/Sub-Folder 1</t>
+          <t>/Python_Admin_Tool_TESTING/Sub-Folder 1/Test Sheet 2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sub-Folder 1</t>
+          <t>Test Sheet 2</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1jPqgww8lNGleK7h15iHuNdyUbZDf0idz</t>
+          <t>1Wan1C_Cxndc2M6yXKa8vxJLXCgYoBXFzDVwRYAfGbVY</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Viewer</t>
+          <t>Commenter</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>user</t>
+          <t>domain</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ernie.moreno62@gmail.com</t>
+          <t>bioaccessla.com</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -701,29 +727,29 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1jPqgww8lNGleK7h15iHuNdyUbZDf0idz</t>
+          <t>https://docs.google.com/spreadsheets/d/1Wan1C_Cxndc2M6yXKa8vxJLXCgYoBXFzDVwRYAfGbVY/edit?usp=drivesdk</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>/Python_Admin_Tool_TESTING/Sub-Folder 1</t>
+          <t>/Python_Admin_Tool_TESTING/Sub-Folder 1/Test Sheet 2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sub-Folder 1</t>
+          <t>Test Sheet 2</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1jPqgww8lNGleK7h15iHuNdyUbZDf0idz</t>
+          <t>1Wan1C_Cxndc2M6yXKa8vxJLXCgYoBXFzDVwRYAfGbVY</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Owner</t>
+          <t>Viewer</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -733,7 +759,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>jmoreno@bioaccessla.com</t>
+          <t>ernie.moreno62@gmail.com</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -743,7 +769,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://drive.google.com/drive/folders/1jPqgww8lNGleK7h15iHuNdyUbZDf0idz</t>
+          <t>https://docs.google.com/spreadsheets/d/1Wan1C_Cxndc2M6yXKa8vxJLXCgYoBXFzDVwRYAfGbVY/edit?usp=drivesdk</t>
         </is>
       </c>
     </row>
@@ -765,7 +791,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Viewer</t>
+          <t>Owner</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -775,7 +801,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>ernie.moreno62@gmail.com</t>
+          <t>jmoreno@bioaccessla.com</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -792,32 +818,32 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>/Python_Admin_Tool_TESTING/Sub-Folder 1/Test Sheet 2</t>
+          <t>/Python_Admin_Tool_TESTING/Test Doc 1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Test Sheet 2</t>
+          <t>Test Doc 1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1Wan1C_Cxndc2M6yXKa8vxJLXCgYoBXFzDVwRYAfGbVY</t>
+          <t>1O90b5jSuK3lIz-RYZIEtAAlA3-IQ_vmxgulyB_6vY2U</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Owner</t>
+          <t>Viewer</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>user</t>
+          <t>domain</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>jmoreno@bioaccessla.com</t>
+          <t>bioaccessla.com</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -827,24 +853,24 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://docs.google.com/spreadsheets/d/1Wan1C_Cxndc2M6yXKa8vxJLXCgYoBXFzDVwRYAfGbVY/edit?usp=drivesdk</t>
+          <t>https://docs.google.com/document/d/1O90b5jSuK3lIz-RYZIEtAAlA3-IQ_vmxgulyB_6vY2U/edit?usp=drivesdk</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>/Python_Admin_Tool_TESTING/Sub-Folder 1/Test Sheet 2</t>
+          <t>/Python_Admin_Tool_TESTING/Test Doc 1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Test Sheet 2</t>
+          <t>Test Doc 1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1Wan1C_Cxndc2M6yXKa8vxJLXCgYoBXFzDVwRYAfGbVY</t>
+          <t>1O90b5jSuK3lIz-RYZIEtAAlA3-IQ_vmxgulyB_6vY2U</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -859,7 +885,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>devassistai@gmail.com</t>
+          <t>ernie.moreno62@gmail.com</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -869,11 +895,64 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://docs.google.com/spreadsheets/d/1Wan1C_Cxndc2M6yXKa8vxJLXCgYoBXFzDVwRYAfGbVY/edit?usp=drivesdk</t>
+          <t>https://docs.google.com/document/d/1O90b5jSuK3lIz-RYZIEtAAlA3-IQ_vmxgulyB_6vY2U/edit?usp=drivesdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>/Python_Admin_Tool_TESTING/Test Doc 1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Test Doc 1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1O90b5jSuK3lIz-RYZIEtAAlA3-IQ_vmxgulyB_6vY2U</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Owner</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>jmoreno@bioaccessla.com</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>jmoreno@bioaccessla.com</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/document/d/1O90b5jSuK3lIz-RYZIEtAAlA3-IQ_vmxgulyB_6vY2U/edit?usp=drivesdk</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:K1048576">
+    <cfRule type="expression" priority="1" dxfId="0">
+      <formula>=$I2="ADD"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="2" dxfId="1">
+      <formula>=$I2="REMOVE"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="3" dxfId="2">
+      <formula>=$I2="MODIFY"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"MODIFY,REMOVE,ADD"</formula1>

</xml_diff>